<commit_message>
Cleaned, loaded travel.xlsx file then created tables into my database londondata.
</commit_message>
<xml_diff>
--- a/LondonDataProject/data/raw/travel.xlsx
+++ b/LondonDataProject/data/raw/travel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamadoucamara/Documents/learning-data-engineering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mahamadoucamara/Documents/Analysis-Of-London-Public-Transportation-System-And-Its-Impact-On-Economic-And-Social/LondonDataProject/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4788E25-01F7-6F48-ADAC-EFBB997D1A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF6B88D-2372-284D-A076-A2CBC3792901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="25" r:id="rId1"/>
@@ -4234,9 +4234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G223"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A208" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G230" sqref="G230"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>